<commit_message>
added greeting functions, default values are populated
</commit_message>
<xml_diff>
--- a/expense_tracker/august.xlsx
+++ b/expense_tracker/august.xlsx
@@ -413,14 +413,32 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Day</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Money Spent</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added skipped edit mode
</commit_message>
<xml_diff>
--- a/expense_tracker/august.xlsx
+++ b/expense_tracker/august.xlsx
@@ -1195,7 +1195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView defaultGridColor="1" showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1242,23 +1242,39 @@
       </c>
     </row>
     <row customHeight="1" ht="16" r="3" s="4">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>18</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>10</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>chips</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="16" r="4" s="4"/>
+    <row customHeight="1" ht="16" r="4" s="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>new shoes</t>
+        </is>
+      </c>
+    </row>
     <row customHeight="1" ht="16" r="5" s="4"/>
     <row customHeight="1" ht="16" r="6" s="4"/>
     <row customHeight="1" ht="16" r="7" s="4"/>

</xml_diff>

<commit_message>
added sum function. acp for the night
</commit_message>
<xml_diff>
--- a/expense_tracker/august.xlsx
+++ b/expense_tracker/august.xlsx
@@ -1195,7 +1195,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView defaultGridColor="1" showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1227,55 +1227,63 @@
     <row customHeight="1" ht="16" r="2" s="4">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>4</t>
         </is>
       </c>
-      <c r="B2" s="1" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="B2" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>new phone</t>
+          <t>fireworks</t>
         </is>
       </c>
     </row>
     <row customHeight="1" ht="16" r="3" s="4">
       <c r="A3" s="1" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>shoes</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="16" r="4" s="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>water</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="16" r="5" s="4">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>18</t>
         </is>
       </c>
-      <c r="B3" s="1" t="inlineStr">
+      <c r="B5" t="n">
+        <v>30</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>watch</t>
         </is>
       </c>
-      <c r="C3" s="1" t="inlineStr">
-        <is>
-          <t>chips</t>
-        </is>
-      </c>
     </row>
-    <row customHeight="1" ht="16" r="4" s="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>new shoes</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="16" r="5" s="4"/>
     <row customHeight="1" ht="16" r="6" s="4"/>
     <row customHeight="1" ht="16" r="7" s="4"/>
     <row customHeight="1" ht="16" r="8" s="4"/>

</xml_diff>